<commit_message>
update, added MoM numbers
</commit_message>
<xml_diff>
--- a/China CPI Solver.xlsx
+++ b/China CPI Solver.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lance\OneDrive\桌面\Coding\China CPI Solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C126D6B6-7524-4ECA-A9B4-A6BC3E257163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDF0036-C1A2-4C60-A540-53AACC2D84F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38303" yWindow="-98" windowWidth="28995" windowHeight="15796" activeTab="1" xr2:uid="{C7829B18-37F2-4AB1-8CCB-E86C5E8B206C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21196" activeTab="1" xr2:uid="{C7829B18-37F2-4AB1-8CCB-E86C5E8B206C}"/>
   </bookViews>
   <sheets>
     <sheet name="YoY" sheetId="1" r:id="rId1"/>
-    <sheet name="Weight" sheetId="2" r:id="rId2"/>
+    <sheet name="MoM" sheetId="3" r:id="rId2"/>
+    <sheet name="Weight" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
   <si>
     <t>Total</t>
   </si>
@@ -444,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90BC7B93-C6A6-4881-B0B2-129B0536B7F8}">
   <dimension ref="A1:J115"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A115"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A79" sqref="A1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4136,11 +4137,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5879B2A-F7CF-4660-B883-A456E7CD568D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC0035B-7D29-475F-9AC3-4EA0DB536FD5}">
   <dimension ref="A1:J115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2:J115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4153,6 +4154,3701 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>42400</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>1.4</v>
+      </c>
+      <c r="D2">
+        <v>-0.37</v>
+      </c>
+      <c r="E2">
+        <v>0.08</v>
+      </c>
+      <c r="F2">
+        <v>0.15</v>
+      </c>
+      <c r="G2">
+        <v>0.04</v>
+      </c>
+      <c r="H2">
+        <v>0.65</v>
+      </c>
+      <c r="I2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>42429</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D3" s="2">
+        <v>-0.35</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>42460</v>
+      </c>
+      <c r="B4">
+        <v>-0.4</v>
+      </c>
+      <c r="C4">
+        <v>-1.3</v>
+      </c>
+      <c r="D4">
+        <v>0.49</v>
+      </c>
+      <c r="E4">
+        <v>0.34</v>
+      </c>
+      <c r="F4">
+        <v>-0.17</v>
+      </c>
+      <c r="G4">
+        <v>-0.69</v>
+      </c>
+      <c r="H4">
+        <v>-0.72</v>
+      </c>
+      <c r="I4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>42490</v>
+      </c>
+      <c r="B5">
+        <v>-0.2</v>
+      </c>
+      <c r="C5">
+        <v>-0.9</v>
+      </c>
+      <c r="D5">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E5">
+        <v>0.16</v>
+      </c>
+      <c r="F5">
+        <v>0.05</v>
+      </c>
+      <c r="G5">
+        <v>0.05</v>
+      </c>
+      <c r="H5">
+        <v>0.12</v>
+      </c>
+      <c r="I5">
+        <v>0.35</v>
+      </c>
+      <c r="J5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>42521</v>
+      </c>
+      <c r="B6">
+        <v>-0.5</v>
+      </c>
+      <c r="C6">
+        <v>-1.8</v>
+      </c>
+      <c r="D6">
+        <v>0.13</v>
+      </c>
+      <c r="E6">
+        <v>0.06</v>
+      </c>
+      <c r="F6">
+        <v>0.02</v>
+      </c>
+      <c r="G6">
+        <v>0.35</v>
+      </c>
+      <c r="H6">
+        <v>-0.1</v>
+      </c>
+      <c r="I6">
+        <v>0.23</v>
+      </c>
+      <c r="J6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>42551</v>
+      </c>
+      <c r="B7">
+        <v>-0.1</v>
+      </c>
+      <c r="C7">
+        <v>-0.9</v>
+      </c>
+      <c r="D7">
+        <v>-0.31</v>
+      </c>
+      <c r="E7">
+        <v>0.1</v>
+      </c>
+      <c r="F7">
+        <v>0.01</v>
+      </c>
+      <c r="G7">
+        <v>0.66</v>
+      </c>
+      <c r="H7">
+        <v>0.32</v>
+      </c>
+      <c r="I7">
+        <v>0.46</v>
+      </c>
+      <c r="J7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>42582</v>
+      </c>
+      <c r="B8">
+        <v>0.2</v>
+      </c>
+      <c r="C8">
+        <v>-0.1</v>
+      </c>
+      <c r="D8">
+        <v>-0.4</v>
+      </c>
+      <c r="E8">
+        <v>0.1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0.1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0.7</v>
+      </c>
+      <c r="J8">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>42613</v>
+      </c>
+      <c r="B9">
+        <v>0.1</v>
+      </c>
+      <c r="C9">
+        <v>0.3</v>
+      </c>
+      <c r="D9">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="E9">
+        <v>0.2</v>
+      </c>
+      <c r="F9">
+        <v>-0.03</v>
+      </c>
+      <c r="G9">
+        <v>-0.63</v>
+      </c>
+      <c r="H9">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="I9">
+        <v>0.33</v>
+      </c>
+      <c r="J9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
+        <v>42643</v>
+      </c>
+      <c r="B10">
+        <v>0.7</v>
+      </c>
+      <c r="C10">
+        <v>1.2</v>
+      </c>
+      <c r="D10">
+        <v>0.8</v>
+      </c>
+      <c r="E10">
+        <v>0.3</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0.3</v>
+      </c>
+      <c r="H10">
+        <v>1.2</v>
+      </c>
+      <c r="I10">
+        <v>0.2</v>
+      </c>
+      <c r="J10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="1">
+        <v>42674</v>
+      </c>
+      <c r="B11">
+        <v>-0.1</v>
+      </c>
+      <c r="C11">
+        <v>-0.6</v>
+      </c>
+      <c r="D11">
+        <v>0.61</v>
+      </c>
+      <c r="E11">
+        <v>0.16</v>
+      </c>
+      <c r="F11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G11">
+        <v>-0.06</v>
+      </c>
+      <c r="H11">
+        <v>-0.32</v>
+      </c>
+      <c r="I11">
+        <v>0.61</v>
+      </c>
+      <c r="J11">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="1">
+        <v>42704</v>
+      </c>
+      <c r="B12">
+        <v>0.1</v>
+      </c>
+      <c r="C12">
+        <v>0.2</v>
+      </c>
+      <c r="D12">
+        <v>0.59</v>
+      </c>
+      <c r="E12">
+        <v>0.23</v>
+      </c>
+      <c r="F12">
+        <v>0.03</v>
+      </c>
+      <c r="G12">
+        <v>0.01</v>
+      </c>
+      <c r="H12">
+        <v>-0.33</v>
+      </c>
+      <c r="I12">
+        <v>0.41</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" s="1">
+        <v>42735</v>
+      </c>
+      <c r="B13">
+        <v>0.2</v>
+      </c>
+      <c r="C13">
+        <v>0.3</v>
+      </c>
+      <c r="D13">
+        <v>-0.13</v>
+      </c>
+      <c r="E13">
+        <v>0.17</v>
+      </c>
+      <c r="F13">
+        <v>0.16</v>
+      </c>
+      <c r="G13">
+        <v>0.53</v>
+      </c>
+      <c r="H13">
+        <v>0.06</v>
+      </c>
+      <c r="I13">
+        <v>0.49</v>
+      </c>
+      <c r="J13">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" s="1">
+        <v>42766</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1.7</v>
+      </c>
+      <c r="D14">
+        <v>-0.45</v>
+      </c>
+      <c r="E14">
+        <v>0.27</v>
+      </c>
+      <c r="F14">
+        <v>0.33</v>
+      </c>
+      <c r="G14">
+        <v>1.44</v>
+      </c>
+      <c r="H14">
+        <v>1.65</v>
+      </c>
+      <c r="I14">
+        <v>0.64</v>
+      </c>
+      <c r="J14">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" s="1">
+        <v>42794</v>
+      </c>
+      <c r="B15">
+        <v>-0.2</v>
+      </c>
+      <c r="C15">
+        <v>-0.3</v>
+      </c>
+      <c r="D15">
+        <v>-0.26</v>
+      </c>
+      <c r="E15">
+        <v>0.41</v>
+      </c>
+      <c r="F15">
+        <v>0.01</v>
+      </c>
+      <c r="G15">
+        <v>-0.41</v>
+      </c>
+      <c r="H15">
+        <v>-0.94</v>
+      </c>
+      <c r="I15">
+        <v>0.26</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" s="1">
+        <v>42825</v>
+      </c>
+      <c r="B16">
+        <v>-0.3</v>
+      </c>
+      <c r="C16">
+        <v>-1.3</v>
+      </c>
+      <c r="D16">
+        <v>0.59</v>
+      </c>
+      <c r="E16">
+        <v>0.24</v>
+      </c>
+      <c r="F16">
+        <v>0.02</v>
+      </c>
+      <c r="G16">
+        <v>-0.36</v>
+      </c>
+      <c r="H16">
+        <v>-0.16</v>
+      </c>
+      <c r="I16">
+        <v>0.48</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" s="1">
+        <v>42855</v>
+      </c>
+      <c r="B17">
+        <v>0.1</v>
+      </c>
+      <c r="C17">
+        <v>-0.3</v>
+      </c>
+      <c r="D17">
+        <v>0.19</v>
+      </c>
+      <c r="E17">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F17">
+        <v>0.23</v>
+      </c>
+      <c r="G17">
+        <v>-0.16</v>
+      </c>
+      <c r="H17">
+        <v>0.35</v>
+      </c>
+      <c r="I17">
+        <v>0.69</v>
+      </c>
+      <c r="J17">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A18" s="1">
+        <v>42886</v>
+      </c>
+      <c r="B18">
+        <v>-0.1</v>
+      </c>
+      <c r="C18">
+        <v>-0.4</v>
+      </c>
+      <c r="D18">
+        <v>0.15</v>
+      </c>
+      <c r="E18">
+        <v>0.11</v>
+      </c>
+      <c r="F18">
+        <v>0.18</v>
+      </c>
+      <c r="G18">
+        <v>-0.31</v>
+      </c>
+      <c r="H18">
+        <v>-0.12</v>
+      </c>
+      <c r="I18">
+        <v>0.37</v>
+      </c>
+      <c r="J18">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A19" s="1">
+        <v>42916</v>
+      </c>
+      <c r="B19">
+        <v>-0.2</v>
+      </c>
+      <c r="C19">
+        <v>-0.7</v>
+      </c>
+      <c r="D19">
+        <v>-0.24</v>
+      </c>
+      <c r="E19">
+        <v>0.15</v>
+      </c>
+      <c r="F19">
+        <v>0.08</v>
+      </c>
+      <c r="G19">
+        <v>-0.31</v>
+      </c>
+      <c r="H19">
+        <v>0.27</v>
+      </c>
+      <c r="I19">
+        <v>0.32</v>
+      </c>
+      <c r="J19">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A20" s="1">
+        <v>42947</v>
+      </c>
+      <c r="B20">
+        <v>0.1</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>-0.43</v>
+      </c>
+      <c r="E20">
+        <v>0.12</v>
+      </c>
+      <c r="F20">
+        <v>0.09</v>
+      </c>
+      <c r="G20">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="H20">
+        <v>0.98</v>
+      </c>
+      <c r="I20">
+        <v>0.52</v>
+      </c>
+      <c r="J20">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A21" s="1">
+        <v>42978</v>
+      </c>
+      <c r="B21">
+        <v>0.4</v>
+      </c>
+      <c r="C21">
+        <v>0.9</v>
+      </c>
+      <c r="D21">
+        <v>-0.21</v>
+      </c>
+      <c r="E21">
+        <v>0.38</v>
+      </c>
+      <c r="F21">
+        <v>0.09</v>
+      </c>
+      <c r="G21">
+        <v>0.32</v>
+      </c>
+      <c r="H21">
+        <v>-0.1</v>
+      </c>
+      <c r="I21">
+        <v>0.74</v>
+      </c>
+      <c r="J21">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A22" s="1">
+        <v>43008</v>
+      </c>
+      <c r="B22">
+        <v>0.5</v>
+      </c>
+      <c r="C22">
+        <v>0.4</v>
+      </c>
+      <c r="D22">
+        <v>0.88</v>
+      </c>
+      <c r="E22">
+        <v>0.34</v>
+      </c>
+      <c r="F22">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G22">
+        <v>0.13</v>
+      </c>
+      <c r="H22">
+        <v>0.95</v>
+      </c>
+      <c r="I22">
+        <v>1.79</v>
+      </c>
+      <c r="J22">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A23" s="1">
+        <v>43039</v>
+      </c>
+      <c r="B23">
+        <v>0.1</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0.54</v>
+      </c>
+      <c r="E23">
+        <v>0.24</v>
+      </c>
+      <c r="F23">
+        <v>0.18</v>
+      </c>
+      <c r="G23">
+        <v>0.24</v>
+      </c>
+      <c r="H23">
+        <v>-0.35</v>
+      </c>
+      <c r="I23">
+        <v>0.24</v>
+      </c>
+      <c r="J23">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A24" s="1">
+        <v>43069</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>-0.3</v>
+      </c>
+      <c r="D24">
+        <v>0.52</v>
+      </c>
+      <c r="E24">
+        <v>0.2</v>
+      </c>
+      <c r="F24">
+        <v>0.09</v>
+      </c>
+      <c r="G24">
+        <v>0.5</v>
+      </c>
+      <c r="H24">
+        <v>-0.54</v>
+      </c>
+      <c r="I24">
+        <v>0.18</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A25" s="1">
+        <v>43100</v>
+      </c>
+      <c r="B25">
+        <v>0.3</v>
+      </c>
+      <c r="C25">
+        <v>0.8</v>
+      </c>
+      <c r="D25">
+        <v>-0.03</v>
+      </c>
+      <c r="E25">
+        <v>0.16</v>
+      </c>
+      <c r="F25">
+        <v>0.21</v>
+      </c>
+      <c r="G25">
+        <v>0.37</v>
+      </c>
+      <c r="H25">
+        <v>0.09</v>
+      </c>
+      <c r="I25">
+        <v>0.15</v>
+      </c>
+      <c r="J25">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A26" s="1">
+        <v>43131</v>
+      </c>
+      <c r="B26">
+        <v>0.6</v>
+      </c>
+      <c r="C26">
+        <v>1.5</v>
+      </c>
+      <c r="D26">
+        <v>-0.35</v>
+      </c>
+      <c r="E26">
+        <v>0.15</v>
+      </c>
+      <c r="F26">
+        <v>0.27</v>
+      </c>
+      <c r="G26">
+        <v>0.45</v>
+      </c>
+      <c r="H26">
+        <v>0.49</v>
+      </c>
+      <c r="I26">
+        <v>0.24</v>
+      </c>
+      <c r="J26">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A27" s="1">
+        <v>43159</v>
+      </c>
+      <c r="B27">
+        <v>1.2</v>
+      </c>
+      <c r="C27">
+        <v>3.1</v>
+      </c>
+      <c r="D27">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0.31</v>
+      </c>
+      <c r="G27">
+        <v>0.94</v>
+      </c>
+      <c r="H27">
+        <v>1.8</v>
+      </c>
+      <c r="I27">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J27">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A28" s="1">
+        <v>43190</v>
+      </c>
+      <c r="B28">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="C28">
+        <v>-2.8</v>
+      </c>
+      <c r="D28">
+        <v>0.6</v>
+      </c>
+      <c r="E28">
+        <v>0.24</v>
+      </c>
+      <c r="F28">
+        <v>-0.21</v>
+      </c>
+      <c r="G28">
+        <v>-1.54</v>
+      </c>
+      <c r="H28">
+        <v>-1.64</v>
+      </c>
+      <c r="I28">
+        <v>0.21</v>
+      </c>
+      <c r="J28">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A29" s="1">
+        <v>43220</v>
+      </c>
+      <c r="B29">
+        <v>-0.2</v>
+      </c>
+      <c r="C29">
+        <v>-1.2</v>
+      </c>
+      <c r="D29">
+        <v>0.18</v>
+      </c>
+      <c r="E29">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F29">
+        <v>0.17</v>
+      </c>
+      <c r="G29">
+        <v>0.62</v>
+      </c>
+      <c r="H29">
+        <v>0.23</v>
+      </c>
+      <c r="I29">
+        <v>0.2</v>
+      </c>
+      <c r="J29">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A30" s="1">
+        <v>43251</v>
+      </c>
+      <c r="B30">
+        <v>-0.2</v>
+      </c>
+      <c r="C30">
+        <v>-0.8</v>
+      </c>
+      <c r="D30">
+        <v>0.2</v>
+      </c>
+      <c r="E30">
+        <v>0.1</v>
+      </c>
+      <c r="F30">
+        <v>0.15</v>
+      </c>
+      <c r="G30">
+        <v>0.37</v>
+      </c>
+      <c r="H30">
+        <v>-0.24</v>
+      </c>
+      <c r="I30">
+        <v>0.25</v>
+      </c>
+      <c r="J30">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A31" s="1">
+        <v>43281</v>
+      </c>
+      <c r="B31">
+        <v>-0.1</v>
+      </c>
+      <c r="C31">
+        <v>-0.5</v>
+      </c>
+      <c r="D31">
+        <v>-0.22</v>
+      </c>
+      <c r="E31">
+        <v>0.18</v>
+      </c>
+      <c r="F31">
+        <v>0.11</v>
+      </c>
+      <c r="G31">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H31">
+        <v>0.2</v>
+      </c>
+      <c r="I31">
+        <v>0.19</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A32" s="1">
+        <v>43312</v>
+      </c>
+      <c r="B32">
+        <v>0.3</v>
+      </c>
+      <c r="C32">
+        <v>0.2</v>
+      </c>
+      <c r="D32">
+        <v>-0.36</v>
+      </c>
+      <c r="E32">
+        <v>0.23</v>
+      </c>
+      <c r="F32">
+        <v>0.12</v>
+      </c>
+      <c r="G32">
+        <v>0.3</v>
+      </c>
+      <c r="H32">
+        <v>1.46</v>
+      </c>
+      <c r="I32">
+        <v>0.22</v>
+      </c>
+      <c r="J32">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A33" s="1">
+        <v>43343</v>
+      </c>
+      <c r="B33">
+        <v>0.7</v>
+      </c>
+      <c r="C33">
+        <v>1.7</v>
+      </c>
+      <c r="D33">
+        <v>-0.09</v>
+      </c>
+      <c r="E33">
+        <v>0.54</v>
+      </c>
+      <c r="F33">
+        <v>0.1</v>
+      </c>
+      <c r="G33">
+        <v>-0.02</v>
+      </c>
+      <c r="H33">
+        <v>0.17</v>
+      </c>
+      <c r="I33">
+        <v>0.4</v>
+      </c>
+      <c r="J33">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A34" s="1">
+        <v>43373</v>
+      </c>
+      <c r="B34">
+        <v>0.7</v>
+      </c>
+      <c r="C34">
+        <v>1.5</v>
+      </c>
+      <c r="D34">
+        <v>0.75</v>
+      </c>
+      <c r="E34">
+        <v>0.39</v>
+      </c>
+      <c r="F34">
+        <v>0.11</v>
+      </c>
+      <c r="G34">
+        <v>0.26</v>
+      </c>
+      <c r="H34">
+        <v>0.52</v>
+      </c>
+      <c r="I34">
+        <v>0.2</v>
+      </c>
+      <c r="J34">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A35" s="1">
+        <v>43404</v>
+      </c>
+      <c r="B35">
+        <v>0.2</v>
+      </c>
+      <c r="C35">
+        <v>-0.1</v>
+      </c>
+      <c r="D35">
+        <v>0.77</v>
+      </c>
+      <c r="E35">
+        <v>0.2</v>
+      </c>
+      <c r="F35">
+        <v>0.1</v>
+      </c>
+      <c r="G35">
+        <v>0.65</v>
+      </c>
+      <c r="H35">
+        <v>-0.04</v>
+      </c>
+      <c r="I35">
+        <v>0.17</v>
+      </c>
+      <c r="J35">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A36" s="1">
+        <v>43434</v>
+      </c>
+      <c r="B36">
+        <v>-0.3</v>
+      </c>
+      <c r="C36">
+        <v>-0.8</v>
+      </c>
+      <c r="D36">
+        <v>0.45</v>
+      </c>
+      <c r="E36">
+        <v>0.05</v>
+      </c>
+      <c r="F36">
+        <v>0.05</v>
+      </c>
+      <c r="G36">
+        <v>-1.03</v>
+      </c>
+      <c r="H36">
+        <v>-0.56000000000000005</v>
+      </c>
+      <c r="I36">
+        <v>0.17</v>
+      </c>
+      <c r="J36">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A37" s="1">
+        <v>43465</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0.8</v>
+      </c>
+      <c r="D37">
+        <v>0.13</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0.18</v>
+      </c>
+      <c r="G37">
+        <v>-1.89</v>
+      </c>
+      <c r="H37">
+        <v>-0.03</v>
+      </c>
+      <c r="I37">
+        <v>0.12</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A38" s="1">
+        <v>43496</v>
+      </c>
+      <c r="B38">
+        <v>0.5</v>
+      </c>
+      <c r="C38">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D38">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="E38">
+        <v>-0.01</v>
+      </c>
+      <c r="F38">
+        <v>0.35</v>
+      </c>
+      <c r="G38">
+        <v>-0.17</v>
+      </c>
+      <c r="H38">
+        <v>1.02</v>
+      </c>
+      <c r="I38">
+        <v>0.36</v>
+      </c>
+      <c r="J38">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A39" s="1">
+        <v>43524</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D39">
+        <v>-0.19</v>
+      </c>
+      <c r="E39">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F39">
+        <v>0.09</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>1.28</v>
+      </c>
+      <c r="I39">
+        <v>0.23</v>
+      </c>
+      <c r="J39">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A40" s="1">
+        <v>43555</v>
+      </c>
+      <c r="B40">
+        <v>-0.4</v>
+      </c>
+      <c r="C40">
+        <v>-0.6</v>
+      </c>
+      <c r="D40">
+        <v>0.61</v>
+      </c>
+      <c r="E40">
+        <v>0.1</v>
+      </c>
+      <c r="F40">
+        <v>-0.34</v>
+      </c>
+      <c r="G40">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="H40">
+        <v>-1.59</v>
+      </c>
+      <c r="I40">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J40">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A41" s="1">
+        <v>43585</v>
+      </c>
+      <c r="B41">
+        <v>0.1</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0.05</v>
+      </c>
+      <c r="E41">
+        <v>0.04</v>
+      </c>
+      <c r="F41">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G41">
+        <v>0.04</v>
+      </c>
+      <c r="H41">
+        <v>0.33</v>
+      </c>
+      <c r="I41">
+        <v>0.1</v>
+      </c>
+      <c r="J41">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A42" s="1">
+        <v>43616</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0.1</v>
+      </c>
+      <c r="D42">
+        <v>0.12</v>
+      </c>
+      <c r="E42">
+        <v>-0.04</v>
+      </c>
+      <c r="F42">
+        <v>0.02</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>-0.17</v>
+      </c>
+      <c r="I42">
+        <v>0.13</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A43" s="1">
+        <v>43646</v>
+      </c>
+      <c r="B43">
+        <v>-0.1</v>
+      </c>
+      <c r="C43">
+        <v>-0.2</v>
+      </c>
+      <c r="D43">
+        <v>-0.1</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>-0.1</v>
+      </c>
+      <c r="G43">
+        <v>-0.7</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0.3</v>
+      </c>
+      <c r="J43">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A44" s="1">
+        <v>43677</v>
+      </c>
+      <c r="B44">
+        <v>0.4</v>
+      </c>
+      <c r="C44">
+        <v>0.7</v>
+      </c>
+      <c r="D44">
+        <v>-0.38</v>
+      </c>
+      <c r="E44">
+        <v>0.09</v>
+      </c>
+      <c r="F44">
+        <v>0.12</v>
+      </c>
+      <c r="G44">
+        <v>0.05</v>
+      </c>
+      <c r="H44">
+        <v>1.32</v>
+      </c>
+      <c r="I44">
+        <v>0.25</v>
+      </c>
+      <c r="J44">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A45" s="1">
+        <v>43708</v>
+      </c>
+      <c r="B45">
+        <v>0.7</v>
+      </c>
+      <c r="C45">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D45">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="E45">
+        <v>0.13</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>-0.23</v>
+      </c>
+      <c r="H45">
+        <v>0.04</v>
+      </c>
+      <c r="I45">
+        <v>0.17</v>
+      </c>
+      <c r="J45">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A46" s="1">
+        <v>43738</v>
+      </c>
+      <c r="B46">
+        <v>0.9</v>
+      </c>
+      <c r="C46">
+        <v>2.6</v>
+      </c>
+      <c r="D46">
+        <v>0.8</v>
+      </c>
+      <c r="E46">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>-0.37</v>
+      </c>
+      <c r="H46">
+        <v>0.15</v>
+      </c>
+      <c r="I46">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J46">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A47" s="1">
+        <v>43769</v>
+      </c>
+      <c r="B47">
+        <v>0.9</v>
+      </c>
+      <c r="C47">
+        <v>2.7</v>
+      </c>
+      <c r="D47">
+        <v>0.31</v>
+      </c>
+      <c r="E47">
+        <v>-0.01</v>
+      </c>
+      <c r="F47">
+        <v>0.08</v>
+      </c>
+      <c r="G47">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H47">
+        <v>0.12</v>
+      </c>
+      <c r="I47">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J47">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A48" s="1">
+        <v>43799</v>
+      </c>
+      <c r="B48">
+        <v>0.4</v>
+      </c>
+      <c r="C48">
+        <v>1.5</v>
+      </c>
+      <c r="D48">
+        <v>0.35</v>
+      </c>
+      <c r="E48">
+        <v>-0.04</v>
+      </c>
+      <c r="F48">
+        <v>-0.09</v>
+      </c>
+      <c r="G48">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="H48">
+        <v>-0.72</v>
+      </c>
+      <c r="I48">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J48">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A49" s="1">
+        <v>43830</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>-0.2</v>
+      </c>
+      <c r="D49">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="E49">
+        <v>0.09</v>
+      </c>
+      <c r="F49">
+        <v>0.11</v>
+      </c>
+      <c r="G49">
+        <v>0.15</v>
+      </c>
+      <c r="H49">
+        <v>0.05</v>
+      </c>
+      <c r="I49">
+        <v>0.17</v>
+      </c>
+      <c r="J49">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A50" s="1">
+        <v>43861</v>
+      </c>
+      <c r="B50">
+        <v>1.4</v>
+      </c>
+      <c r="C50">
+        <v>3.1</v>
+      </c>
+      <c r="D50">
+        <v>-0.53</v>
+      </c>
+      <c r="E50">
+        <v>-0.02</v>
+      </c>
+      <c r="F50">
+        <v>0.22</v>
+      </c>
+      <c r="G50">
+        <v>1.44</v>
+      </c>
+      <c r="H50">
+        <v>1.43</v>
+      </c>
+      <c r="I50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="J50">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A51" s="1">
+        <v>43890</v>
+      </c>
+      <c r="B51">
+        <v>0.8</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51">
+        <v>-0.27</v>
+      </c>
+      <c r="E51">
+        <v>-0.11</v>
+      </c>
+      <c r="F51">
+        <v>-0.08</v>
+      </c>
+      <c r="G51">
+        <v>-1.46</v>
+      </c>
+      <c r="H51">
+        <v>0.02</v>
+      </c>
+      <c r="I51">
+        <v>0.12</v>
+      </c>
+      <c r="J51">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A52" s="1">
+        <v>43921</v>
+      </c>
+      <c r="B52">
+        <v>-1.2</v>
+      </c>
+      <c r="C52">
+        <v>-2.7</v>
+      </c>
+      <c r="D52">
+        <v>-0.15</v>
+      </c>
+      <c r="E52">
+        <v>-0.27</v>
+      </c>
+      <c r="F52">
+        <v>-0.13</v>
+      </c>
+      <c r="G52">
+        <v>-2.46</v>
+      </c>
+      <c r="H52">
+        <v>-0.05</v>
+      </c>
+      <c r="I52">
+        <v>0.16</v>
+      </c>
+      <c r="J52">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A53" s="1">
+        <v>43951</v>
+      </c>
+      <c r="B53">
+        <v>-0.9</v>
+      </c>
+      <c r="C53">
+        <v>-2.1</v>
+      </c>
+      <c r="D53">
+        <v>-0.06</v>
+      </c>
+      <c r="E53">
+        <v>-0.18</v>
+      </c>
+      <c r="F53">
+        <v>-0.09</v>
+      </c>
+      <c r="G53">
+        <v>-1.18</v>
+      </c>
+      <c r="H53">
+        <v>-0.19</v>
+      </c>
+      <c r="I53">
+        <v>0.17</v>
+      </c>
+      <c r="J53">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A54" s="1">
+        <v>43982</v>
+      </c>
+      <c r="B54">
+        <v>-0.8</v>
+      </c>
+      <c r="C54">
+        <v>-2.4</v>
+      </c>
+      <c r="D54">
+        <v>0.15</v>
+      </c>
+      <c r="E54">
+        <v>-0.17</v>
+      </c>
+      <c r="F54">
+        <v>0.01</v>
+      </c>
+      <c r="G54">
+        <v>-0.16</v>
+      </c>
+      <c r="H54">
+        <v>0.03</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A55" s="1">
+        <v>44012</v>
+      </c>
+      <c r="B55">
+        <v>-0.1</v>
+      </c>
+      <c r="C55">
+        <v>0.1</v>
+      </c>
+      <c r="D55">
+        <v>-0.22</v>
+      </c>
+      <c r="E55">
+        <v>-0.17</v>
+      </c>
+      <c r="F55">
+        <v>-0.12</v>
+      </c>
+      <c r="G55">
+        <v>-0.25</v>
+      </c>
+      <c r="H55">
+        <v>-0.27</v>
+      </c>
+      <c r="I55">
+        <v>0.01</v>
+      </c>
+      <c r="J55">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A56" s="1">
+        <v>44043</v>
+      </c>
+      <c r="B56">
+        <v>0.6</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56">
+        <v>-0.5</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0.3</v>
+      </c>
+      <c r="H56">
+        <v>-0.2</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A57" s="1">
+        <v>44074</v>
+      </c>
+      <c r="B57">
+        <v>0.4</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>-0.2</v>
+      </c>
+      <c r="E57">
+        <v>0.1</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0.3</v>
+      </c>
+      <c r="H57">
+        <v>-0.3</v>
+      </c>
+      <c r="I57">
+        <v>0.1</v>
+      </c>
+      <c r="J57">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A58" s="1">
+        <v>44104</v>
+      </c>
+      <c r="B58">
+        <v>0.2</v>
+      </c>
+      <c r="C58">
+        <v>0.3</v>
+      </c>
+      <c r="D58">
+        <v>0.9</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>-0.1</v>
+      </c>
+      <c r="H58">
+        <v>0.8</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A59" s="1">
+        <v>44135</v>
+      </c>
+      <c r="B59">
+        <v>-0.3</v>
+      </c>
+      <c r="C59">
+        <v>-1.2</v>
+      </c>
+      <c r="D59">
+        <v>0.4</v>
+      </c>
+      <c r="E59">
+        <v>0.1</v>
+      </c>
+      <c r="F59">
+        <v>0.1</v>
+      </c>
+      <c r="G59">
+        <v>-0.2</v>
+      </c>
+      <c r="H59">
+        <v>0.6</v>
+      </c>
+      <c r="I59">
+        <v>0.1</v>
+      </c>
+      <c r="J59">
+        <v>-1.7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A60" s="1">
+        <v>44165</v>
+      </c>
+      <c r="B60">
+        <v>-0.6</v>
+      </c>
+      <c r="C60">
+        <v>-1.6</v>
+      </c>
+      <c r="D60">
+        <v>0.3</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>-0.3</v>
+      </c>
+      <c r="H60">
+        <v>-0.8</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A61" s="1">
+        <v>44196</v>
+      </c>
+      <c r="B61">
+        <v>0.7</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0.1</v>
+      </c>
+      <c r="F61">
+        <v>0.1</v>
+      </c>
+      <c r="G61">
+        <v>0.9</v>
+      </c>
+      <c r="H61">
+        <v>-0.1</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A62" s="1">
+        <v>44227</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>2.8</v>
+      </c>
+      <c r="D62">
+        <v>-0.4</v>
+      </c>
+      <c r="E62">
+        <v>0.1</v>
+      </c>
+      <c r="F62">
+        <v>0.2</v>
+      </c>
+      <c r="G62">
+        <v>0.9</v>
+      </c>
+      <c r="H62">
+        <v>0.4</v>
+      </c>
+      <c r="I62">
+        <v>0.1</v>
+      </c>
+      <c r="J62">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A63" s="1">
+        <v>44255</v>
+      </c>
+      <c r="B63">
+        <v>0.6</v>
+      </c>
+      <c r="C63">
+        <v>1.2</v>
+      </c>
+      <c r="D63">
+        <v>-0.5</v>
+      </c>
+      <c r="E63">
+        <v>0.1</v>
+      </c>
+      <c r="F63">
+        <v>0.1</v>
+      </c>
+      <c r="G63">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H63">
+        <v>0.8</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A64" s="1">
+        <v>44286</v>
+      </c>
+      <c r="B64">
+        <v>-0.5</v>
+      </c>
+      <c r="C64">
+        <v>-2.4</v>
+      </c>
+      <c r="D64">
+        <v>0.4</v>
+      </c>
+      <c r="E64">
+        <v>0.2</v>
+      </c>
+      <c r="F64">
+        <v>-0.1</v>
+      </c>
+      <c r="G64">
+        <v>1.3</v>
+      </c>
+      <c r="H64">
+        <v>-0.4</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A65" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B65">
+        <v>-0.3</v>
+      </c>
+      <c r="C65">
+        <v>-1.5</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0.1</v>
+      </c>
+      <c r="F65">
+        <v>0.3</v>
+      </c>
+      <c r="G65">
+        <v>0.4</v>
+      </c>
+      <c r="H65">
+        <v>0.7</v>
+      </c>
+      <c r="I65">
+        <v>0.1</v>
+      </c>
+      <c r="J65">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A66" s="1">
+        <v>44347</v>
+      </c>
+      <c r="B66">
+        <v>-0.2</v>
+      </c>
+      <c r="C66">
+        <v>-1</v>
+      </c>
+      <c r="D66">
+        <v>0.3</v>
+      </c>
+      <c r="E66">
+        <v>0.1</v>
+      </c>
+      <c r="F66">
+        <v>-0.1</v>
+      </c>
+      <c r="G66">
+        <v>0.4</v>
+      </c>
+      <c r="H66">
+        <v>0.3</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A67" s="1">
+        <v>44377</v>
+      </c>
+      <c r="B67">
+        <v>-0.4</v>
+      </c>
+      <c r="C67">
+        <v>-1.4</v>
+      </c>
+      <c r="D67">
+        <v>-0.2</v>
+      </c>
+      <c r="E67">
+        <v>0.1</v>
+      </c>
+      <c r="F67">
+        <v>-0.2</v>
+      </c>
+      <c r="G67">
+        <v>0.1</v>
+      </c>
+      <c r="H67">
+        <v>-0.2</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A68" s="1">
+        <v>44408</v>
+      </c>
+      <c r="B68">
+        <v>0.3</v>
+      </c>
+      <c r="C68">
+        <v>-0.2</v>
+      </c>
+      <c r="D68">
+        <v>-0.4</v>
+      </c>
+      <c r="E68">
+        <v>0.2</v>
+      </c>
+      <c r="F68">
+        <v>0.4</v>
+      </c>
+      <c r="G68">
+        <v>1.5</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>0.1</v>
+      </c>
+      <c r="J68">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A69" s="1">
+        <v>44439</v>
+      </c>
+      <c r="B69">
+        <v>0.1</v>
+      </c>
+      <c r="C69">
+        <v>0.5</v>
+      </c>
+      <c r="D69">
+        <v>-0.1</v>
+      </c>
+      <c r="E69">
+        <v>0.1</v>
+      </c>
+      <c r="F69">
+        <v>0.1</v>
+      </c>
+      <c r="G69">
+        <v>-0.6</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A70" s="1">
+        <v>44469</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>-0.4</v>
+      </c>
+      <c r="D70">
+        <v>0.8</v>
+      </c>
+      <c r="E70">
+        <v>0.2</v>
+      </c>
+      <c r="F70">
+        <v>-0.1</v>
+      </c>
+      <c r="G70">
+        <v>-0.2</v>
+      </c>
+      <c r="H70">
+        <v>0.7</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A71" s="1">
+        <v>44500</v>
+      </c>
+      <c r="B71">
+        <v>0.7</v>
+      </c>
+      <c r="C71">
+        <v>1.2</v>
+      </c>
+      <c r="D71">
+        <v>0.3</v>
+      </c>
+      <c r="E71">
+        <v>0.4</v>
+      </c>
+      <c r="F71">
+        <v>0.3</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>0.2</v>
+      </c>
+      <c r="I71">
+        <v>0.2</v>
+      </c>
+      <c r="J71">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A72" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B72">
+        <v>0.4</v>
+      </c>
+      <c r="C72">
+        <v>1.6</v>
+      </c>
+      <c r="D72">
+        <v>0.3</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>-0.4</v>
+      </c>
+      <c r="G72">
+        <v>0.3</v>
+      </c>
+      <c r="H72">
+        <v>-0.5</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A73" s="1">
+        <v>44561</v>
+      </c>
+      <c r="B73">
+        <v>-0.3</v>
+      </c>
+      <c r="C73">
+        <v>-0.3</v>
+      </c>
+      <c r="D73">
+        <v>0.1</v>
+      </c>
+      <c r="E73">
+        <v>-0.1</v>
+      </c>
+      <c r="F73">
+        <v>0.3</v>
+      </c>
+      <c r="G73">
+        <v>-1.3</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A74" s="1">
+        <v>44592</v>
+      </c>
+      <c r="B74">
+        <v>0.4</v>
+      </c>
+      <c r="C74">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D74">
+        <v>-0.5</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>-0.1</v>
+      </c>
+      <c r="G74">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H74">
+        <v>0.2</v>
+      </c>
+      <c r="I74">
+        <v>0.1</v>
+      </c>
+      <c r="J74">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A75" s="1">
+        <v>44620</v>
+      </c>
+      <c r="B75">
+        <v>0.6</v>
+      </c>
+      <c r="C75">
+        <v>1.2</v>
+      </c>
+      <c r="D75">
+        <v>-0.3</v>
+      </c>
+      <c r="E75">
+        <v>0.1</v>
+      </c>
+      <c r="F75">
+        <v>0.2</v>
+      </c>
+      <c r="G75">
+        <v>1.4</v>
+      </c>
+      <c r="H75">
+        <v>0.4</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A76" s="1">
+        <v>44651</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>-0.9</v>
+      </c>
+      <c r="D76">
+        <v>0.4</v>
+      </c>
+      <c r="E76">
+        <v>0.1</v>
+      </c>
+      <c r="F76">
+        <v>0.2</v>
+      </c>
+      <c r="G76">
+        <v>1.6</v>
+      </c>
+      <c r="H76">
+        <v>-0.3</v>
+      </c>
+      <c r="I76">
+        <v>0.1</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A77" s="1">
+        <v>44681</v>
+      </c>
+      <c r="B77">
+        <v>0.4</v>
+      </c>
+      <c r="C77">
+        <v>0.7</v>
+      </c>
+      <c r="D77">
+        <v>-0.2</v>
+      </c>
+      <c r="E77">
+        <v>-0.1</v>
+      </c>
+      <c r="F77">
+        <v>0.6</v>
+      </c>
+      <c r="G77">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H77">
+        <v>0.1</v>
+      </c>
+      <c r="I77">
+        <v>0.1</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A78" s="1">
+        <v>44712</v>
+      </c>
+      <c r="B78">
+        <v>-0.2</v>
+      </c>
+      <c r="C78">
+        <v>-0.9</v>
+      </c>
+      <c r="D78">
+        <v>0.4</v>
+      </c>
+      <c r="E78">
+        <v>-0.1</v>
+      </c>
+      <c r="F78">
+        <v>0.2</v>
+      </c>
+      <c r="G78">
+        <v>0.1</v>
+      </c>
+      <c r="H78">
+        <v>0.1</v>
+      </c>
+      <c r="I78">
+        <v>0.1</v>
+      </c>
+      <c r="J78">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A79" s="1">
+        <v>44742</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>-1</v>
+      </c>
+      <c r="D79">
+        <v>-0.1</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>-0.2</v>
+      </c>
+      <c r="G79">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H79">
+        <v>0.1</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A80" s="1">
+        <v>44773</v>
+      </c>
+      <c r="B80">
+        <v>0.5</v>
+      </c>
+      <c r="C80">
+        <v>1.9</v>
+      </c>
+      <c r="D80">
+        <v>-0.4</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0.3</v>
+      </c>
+      <c r="G80">
+        <v>-0.7</v>
+      </c>
+      <c r="H80">
+        <v>0.5</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A81" s="1">
+        <v>44804</v>
+      </c>
+      <c r="B81">
+        <v>-0.1</v>
+      </c>
+      <c r="C81">
+        <v>0.4</v>
+      </c>
+      <c r="D81">
+        <v>-0.2</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>-1.7</v>
+      </c>
+      <c r="H81">
+        <v>0.1</v>
+      </c>
+      <c r="I81">
+        <v>0.1</v>
+      </c>
+      <c r="J81">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A82" s="1">
+        <v>44834</v>
+      </c>
+      <c r="B82">
+        <v>0.3</v>
+      </c>
+      <c r="C82">
+        <v>1.3</v>
+      </c>
+      <c r="D82">
+        <v>0.8</v>
+      </c>
+      <c r="E82">
+        <v>-0.1</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>-0.6</v>
+      </c>
+      <c r="H82">
+        <v>0.4</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+      <c r="J82">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A83" s="1">
+        <v>44865</v>
+      </c>
+      <c r="B83">
+        <v>0.1</v>
+      </c>
+      <c r="C83">
+        <v>0.2</v>
+      </c>
+      <c r="D83">
+        <v>0.3</v>
+      </c>
+      <c r="E83">
+        <v>-0.1</v>
+      </c>
+      <c r="F83">
+        <v>0.3</v>
+      </c>
+      <c r="G83">
+        <v>-0.4</v>
+      </c>
+      <c r="H83">
+        <v>0.2</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A84" s="1">
+        <v>44895</v>
+      </c>
+      <c r="B84">
+        <v>-0.2</v>
+      </c>
+      <c r="C84">
+        <v>-0.5</v>
+      </c>
+      <c r="D84">
+        <v>0.3</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>-0.3</v>
+      </c>
+      <c r="G84">
+        <v>0.1</v>
+      </c>
+      <c r="H84">
+        <v>-0.4</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A85" s="1">
+        <v>44926</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>0.4</v>
+      </c>
+      <c r="D85">
+        <v>0.1</v>
+      </c>
+      <c r="E85">
+        <v>-0.1</v>
+      </c>
+      <c r="F85">
+        <v>0.3</v>
+      </c>
+      <c r="G85">
+        <v>-1.4</v>
+      </c>
+      <c r="H85">
+        <v>0.1</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A86" s="1">
+        <v>44957</v>
+      </c>
+      <c r="B86">
+        <v>0.8</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86">
+        <v>-0.5</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>0.2</v>
+      </c>
+      <c r="H86">
+        <v>1.3</v>
+      </c>
+      <c r="I86">
+        <v>0.3</v>
+      </c>
+      <c r="J86">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A87" s="1">
+        <v>44985</v>
+      </c>
+      <c r="B87">
+        <v>-0.5</v>
+      </c>
+      <c r="C87">
+        <v>-1.3</v>
+      </c>
+      <c r="D87">
+        <v>-0.1</v>
+      </c>
+      <c r="E87">
+        <v>0.1</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>-0.5</v>
+      </c>
+      <c r="H87">
+        <v>-0.8</v>
+      </c>
+      <c r="I87">
+        <v>0.2</v>
+      </c>
+      <c r="J87">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A88" s="1">
+        <v>45016</v>
+      </c>
+      <c r="B88">
+        <v>-0.3</v>
+      </c>
+      <c r="C88">
+        <v>-0.9</v>
+      </c>
+      <c r="D88">
+        <v>0.5</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>-0.5</v>
+      </c>
+      <c r="G88">
+        <v>-0.4</v>
+      </c>
+      <c r="H88">
+        <v>-0.1</v>
+      </c>
+      <c r="I88">
+        <v>0.1</v>
+      </c>
+      <c r="J88">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A89" s="1">
+        <v>45046</v>
+      </c>
+      <c r="B89">
+        <v>-0.1</v>
+      </c>
+      <c r="C89">
+        <v>-0.6</v>
+      </c>
+      <c r="D89">
+        <v>-0.1</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>-0.4</v>
+      </c>
+      <c r="H89">
+        <v>0.5</v>
+      </c>
+      <c r="I89">
+        <v>0.1</v>
+      </c>
+      <c r="J89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A90" s="1">
+        <v>45077</v>
+      </c>
+      <c r="B90">
+        <v>-0.2</v>
+      </c>
+      <c r="C90">
+        <v>-0.4</v>
+      </c>
+      <c r="D90">
+        <v>0.4</v>
+      </c>
+      <c r="E90">
+        <v>-0.1</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>-0.6</v>
+      </c>
+      <c r="H90">
+        <v>-0.1</v>
+      </c>
+      <c r="I90">
+        <v>0.1</v>
+      </c>
+      <c r="J90">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A91" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B91">
+        <v>-0.2</v>
+      </c>
+      <c r="C91">
+        <v>-0.2</v>
+      </c>
+      <c r="D91">
+        <v>-0.2</v>
+      </c>
+      <c r="E91">
+        <v>0.1</v>
+      </c>
+      <c r="F91">
+        <v>-0.5</v>
+      </c>
+      <c r="G91">
+        <v>-0.5</v>
+      </c>
+      <c r="H91">
+        <v>-0.2</v>
+      </c>
+      <c r="I91">
+        <v>0.1</v>
+      </c>
+      <c r="J91">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A92" s="1">
+        <v>45138</v>
+      </c>
+      <c r="B92">
+        <v>0.2</v>
+      </c>
+      <c r="C92">
+        <v>-0.6</v>
+      </c>
+      <c r="D92">
+        <v>-0.3</v>
+      </c>
+      <c r="E92">
+        <v>0.1</v>
+      </c>
+      <c r="F92">
+        <v>0.6</v>
+      </c>
+      <c r="G92">
+        <v>1.2</v>
+      </c>
+      <c r="H92">
+        <v>1.3</v>
+      </c>
+      <c r="I92">
+        <v>0.1</v>
+      </c>
+      <c r="J92">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A93" s="1">
+        <v>45169</v>
+      </c>
+      <c r="B93">
+        <v>0.3</v>
+      </c>
+      <c r="C93">
+        <v>0.4</v>
+      </c>
+      <c r="D93">
+        <v>-0.1</v>
+      </c>
+      <c r="E93">
+        <v>0.1</v>
+      </c>
+      <c r="F93">
+        <v>-0.3</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+      <c r="H93">
+        <v>0.2</v>
+      </c>
+      <c r="I93">
+        <v>0.1</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A94" s="1">
+        <v>45199</v>
+      </c>
+      <c r="B94">
+        <v>0.2</v>
+      </c>
+      <c r="C94">
+        <v>0.2</v>
+      </c>
+      <c r="D94">
+        <v>0.8</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>0.1</v>
+      </c>
+      <c r="G94">
+        <v>0.1</v>
+      </c>
+      <c r="H94">
+        <v>0.4</v>
+      </c>
+      <c r="I94">
+        <v>0.1</v>
+      </c>
+      <c r="J94">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A95" s="1">
+        <v>45230</v>
+      </c>
+      <c r="B95">
+        <v>-0.1</v>
+      </c>
+      <c r="C95">
+        <v>-0.4</v>
+      </c>
+      <c r="D95">
+        <v>0.2</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>0.1</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
+      </c>
+      <c r="J95">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A96" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B96">
+        <v>-0.5</v>
+      </c>
+      <c r="C96">
+        <v>-0.6</v>
+      </c>
+      <c r="D96">
+        <v>0.6</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>-0.2</v>
+      </c>
+      <c r="G96">
+        <v>-1.4</v>
+      </c>
+      <c r="H96">
+        <v>-0.9</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+      <c r="J96">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A97" s="1">
+        <v>45291</v>
+      </c>
+      <c r="B97">
+        <v>0.1</v>
+      </c>
+      <c r="C97">
+        <v>0.6</v>
+      </c>
+      <c r="D97">
+        <v>0.1</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0.8</v>
+      </c>
+      <c r="G97">
+        <v>-1.2</v>
+      </c>
+      <c r="H97">
+        <v>0.1</v>
+      </c>
+      <c r="I97">
+        <v>0.1</v>
+      </c>
+      <c r="J97">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A98" s="1">
+        <v>45322</v>
+      </c>
+      <c r="B98">
+        <v>0.3</v>
+      </c>
+      <c r="C98">
+        <v>0.3</v>
+      </c>
+      <c r="D98">
+        <v>-0.3</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+      <c r="G98">
+        <v>0.1</v>
+      </c>
+      <c r="H98">
+        <v>0.7</v>
+      </c>
+      <c r="I98">
+        <v>0.1</v>
+      </c>
+      <c r="J98">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A99" s="1">
+        <v>45351</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="C99">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D99">
+        <v>-0.2</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>-0.5</v>
+      </c>
+      <c r="G99">
+        <v>1.6</v>
+      </c>
+      <c r="H99">
+        <v>1.7</v>
+      </c>
+      <c r="I99">
+        <v>0.4</v>
+      </c>
+      <c r="J99">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A100" s="1">
+        <v>45382</v>
+      </c>
+      <c r="B100">
+        <v>-1</v>
+      </c>
+      <c r="C100">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="D100">
+        <v>0.6</v>
+      </c>
+      <c r="E100">
+        <v>0.1</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>-1.4</v>
+      </c>
+      <c r="H100">
+        <v>-2.1</v>
+      </c>
+      <c r="I100">
+        <v>0.1</v>
+      </c>
+      <c r="J100">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A101" s="1">
+        <v>45412</v>
+      </c>
+      <c r="B101">
+        <v>0.1</v>
+      </c>
+      <c r="C101">
+        <v>-0.7</v>
+      </c>
+      <c r="D101">
+        <v>-0.1</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>0.4</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
+      </c>
+      <c r="H101">
+        <v>0.5</v>
+      </c>
+      <c r="I101">
+        <v>0.2</v>
+      </c>
+      <c r="J101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A102" s="1">
+        <v>45443</v>
+      </c>
+      <c r="B102">
+        <v>-0.1</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>0.4</v>
+      </c>
+      <c r="E102">
+        <v>-0.1</v>
+      </c>
+      <c r="F102">
+        <v>-0.7</v>
+      </c>
+      <c r="G102">
+        <v>-0.8</v>
+      </c>
+      <c r="H102">
+        <v>-0.1</v>
+      </c>
+      <c r="I102">
+        <v>0</v>
+      </c>
+      <c r="J102">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A103" s="1">
+        <v>45473</v>
+      </c>
+      <c r="B103">
+        <v>-0.2</v>
+      </c>
+      <c r="C103">
+        <v>-0.4</v>
+      </c>
+      <c r="D103">
+        <v>-0.2</v>
+      </c>
+      <c r="E103">
+        <v>0.1</v>
+      </c>
+      <c r="F103">
+        <v>-0.4</v>
+      </c>
+      <c r="G103">
+        <v>-0.6</v>
+      </c>
+      <c r="H103">
+        <v>-0.2</v>
+      </c>
+      <c r="I103">
+        <v>0.1</v>
+      </c>
+      <c r="J103">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A104" s="1">
+        <v>45504</v>
+      </c>
+      <c r="B104">
+        <v>0.5</v>
+      </c>
+      <c r="C104">
+        <v>0.7</v>
+      </c>
+      <c r="D104">
+        <v>-0.4</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <v>0.4</v>
+      </c>
+      <c r="G104">
+        <v>0.9</v>
+      </c>
+      <c r="H104">
+        <v>1.3</v>
+      </c>
+      <c r="I104">
+        <v>0</v>
+      </c>
+      <c r="J104">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A105" s="1">
+        <v>45535</v>
+      </c>
+      <c r="B105">
+        <v>0.4</v>
+      </c>
+      <c r="C105">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D105">
+        <v>-0.2</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105">
+        <v>-0.7</v>
+      </c>
+      <c r="G105">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="H105">
+        <v>-0.1</v>
+      </c>
+      <c r="I105">
+        <v>0</v>
+      </c>
+      <c r="J105">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A106" s="1">
+        <v>45565</v>
+      </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
+      <c r="C106">
+        <v>0.5</v>
+      </c>
+      <c r="D106">
+        <v>0.8</v>
+      </c>
+      <c r="E106">
+        <v>-0.1</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+      <c r="G106">
+        <v>-1.3</v>
+      </c>
+      <c r="H106">
+        <v>-0.3</v>
+      </c>
+      <c r="I106">
+        <v>0</v>
+      </c>
+      <c r="J106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A107" s="1">
+        <v>45596</v>
+      </c>
+      <c r="B107">
+        <v>-0.3</v>
+      </c>
+      <c r="C107">
+        <v>-0.8</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107">
+        <v>0.1</v>
+      </c>
+      <c r="G107">
+        <v>-0.7</v>
+      </c>
+      <c r="H107">
+        <v>0.2</v>
+      </c>
+      <c r="I107">
+        <v>0</v>
+      </c>
+      <c r="J107">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A108" s="1">
+        <v>45626</v>
+      </c>
+      <c r="B108">
+        <v>-0.6</v>
+      </c>
+      <c r="C108">
+        <v>-1.7</v>
+      </c>
+      <c r="D108">
+        <v>0.6</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <v>-0.6</v>
+      </c>
+      <c r="G108">
+        <v>-0.1</v>
+      </c>
+      <c r="H108">
+        <v>-0.7</v>
+      </c>
+      <c r="I108">
+        <v>0</v>
+      </c>
+      <c r="J108">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A109" s="1">
+        <v>45657</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+      <c r="C109">
+        <v>-0.3</v>
+      </c>
+      <c r="D109">
+        <v>0.2</v>
+      </c>
+      <c r="E109">
+        <v>0.1</v>
+      </c>
+      <c r="F109">
+        <v>0.3</v>
+      </c>
+      <c r="G109">
+        <v>0.3</v>
+      </c>
+      <c r="H109">
+        <v>0</v>
+      </c>
+      <c r="I109">
+        <v>-0.1</v>
+      </c>
+      <c r="J109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A110" s="1">
+        <v>45688</v>
+      </c>
+      <c r="B110">
+        <v>0.7</v>
+      </c>
+      <c r="C110">
+        <v>0.9</v>
+      </c>
+      <c r="D110">
+        <v>-0.4</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110">
+        <v>0.7</v>
+      </c>
+      <c r="G110">
+        <v>1.7</v>
+      </c>
+      <c r="H110">
+        <v>1.5</v>
+      </c>
+      <c r="I110">
+        <v>0</v>
+      </c>
+      <c r="J110">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A111" s="1">
+        <v>45716</v>
+      </c>
+      <c r="B111">
+        <v>-0.2</v>
+      </c>
+      <c r="C111">
+        <v>-0.2</v>
+      </c>
+      <c r="D111">
+        <v>-0.1</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="F111">
+        <v>-0.1</v>
+      </c>
+      <c r="G111">
+        <v>-0.4</v>
+      </c>
+      <c r="H111">
+        <v>-0.5</v>
+      </c>
+      <c r="I111">
+        <v>0</v>
+      </c>
+      <c r="J111">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A112" s="1">
+        <v>45747</v>
+      </c>
+      <c r="B112">
+        <v>-0.4</v>
+      </c>
+      <c r="C112">
+        <v>-0.9</v>
+      </c>
+      <c r="D112">
+        <v>0.7</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <v>1.3</v>
+      </c>
+      <c r="G112">
+        <v>-1.4</v>
+      </c>
+      <c r="H112">
+        <v>-0.8</v>
+      </c>
+      <c r="I112">
+        <v>0</v>
+      </c>
+      <c r="J112">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A113" s="1">
+        <v>45777</v>
+      </c>
+      <c r="B113">
+        <v>0.1</v>
+      </c>
+      <c r="C113">
+        <v>0.2</v>
+      </c>
+      <c r="D113">
+        <v>-0.1</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+      <c r="G113">
+        <v>-0.3</v>
+      </c>
+      <c r="H113">
+        <v>0.4</v>
+      </c>
+      <c r="I113">
+        <v>0.2</v>
+      </c>
+      <c r="J113">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A114" s="1">
+        <v>45808</v>
+      </c>
+      <c r="B114">
+        <v>-0.2</v>
+      </c>
+      <c r="C114">
+        <v>-0.2</v>
+      </c>
+      <c r="D114">
+        <v>0.6</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="F114">
+        <v>-0.8</v>
+      </c>
+      <c r="G114">
+        <v>-1.2</v>
+      </c>
+      <c r="H114">
+        <v>0.1</v>
+      </c>
+      <c r="I114">
+        <v>0.1</v>
+      </c>
+      <c r="J114">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A115" s="1">
+        <v>45838</v>
+      </c>
+      <c r="B115">
+        <v>-0.1</v>
+      </c>
+      <c r="C115">
+        <v>-0.3</v>
+      </c>
+      <c r="D115">
+        <v>-0.1</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <v>0.2</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>-0.1</v>
+      </c>
+      <c r="I115">
+        <v>0.1</v>
+      </c>
+      <c r="J115">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5879B2A-F7CF-4660-B883-A456E7CD568D}">
+  <dimension ref="A1:J115"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">

</xml_diff>